<commit_message>
Ran some tests, simplified GetTransactionItem
</commit_message>
<xml_diff>
--- a/REFGoogleScholar/Data/Config.xlsx
+++ b/REFGoogleScholar/Data/Config.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paul/UBB/rpa/RPA_project/REFGoogleScholar/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ANDREI\source\repos\GitHub_Desktop_repos\RPA_project\REFGoogleScholar\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AB5A8A3-6282-E445-B761-FA69A9531FFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="33600" windowHeight="20400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="33600" windowHeight="20400"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -189,7 +188,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -272,9 +271,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -312,7 +311,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -418,7 +417,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -560,29 +559,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="43.5" customWidth="1"/>
+    <col min="1" max="1" width="43.44140625" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.5" customWidth="1"/>
+    <col min="3" max="3" width="81.44140625" customWidth="1"/>
     <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="19">
+    <row r="1" spans="1:26" ht="18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -627,7 +626,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="32">
+    <row r="3" spans="1:26" ht="43.2">
       <c r="A3" s="2" t="s">
         <v>37</v>
       </c>
@@ -641,7 +640,7 @@
     <row r="4" spans="1:26">
       <c r="A4" s="2"/>
     </row>
-    <row r="5" spans="1:26" ht="32">
+    <row r="5" spans="1:26" ht="28.8">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -683,9 +682,9 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C6" r:id="rId2" display="https://scholar.google.com/" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="C7" r:id="rId3" display="mailto:your.email@gmail.com" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B6" r:id="rId1"/>
+    <hyperlink ref="C6" r:id="rId2" display="https://scholar.google.com/"/>
+    <hyperlink ref="C7" r:id="rId3" display="mailto:your.email@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -693,22 +692,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.5" customWidth="1"/>
+    <col min="3" max="3" width="75.44140625" customWidth="1"/>
     <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="19">
+    <row r="1" spans="1:26" ht="18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -742,7 +741,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="32">
+    <row r="2" spans="1:26" ht="28.8">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -753,7 +752,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="32">
+    <row r="3" spans="1:26" ht="43.2">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -866,7 +865,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="32">
+    <row r="17" spans="1:3" ht="28.8">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -884,19 +883,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.83203125" customWidth="1"/>
-    <col min="2" max="2" width="30.1640625" customWidth="1"/>
+    <col min="1" max="1" width="31.77734375" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" customWidth="1"/>
     <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.5" customWidth="1"/>
+    <col min="4" max="26" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>